<commit_message>
Rearrange S Tables on 240725
</commit_message>
<xml_diff>
--- a/SI_Tables/Table_#15.xlsx
+++ b/SI_Tables/Table_#15.xlsx
@@ -1,26 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\431_VscRNAseq__PBMC_analysis\003_cWF_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tns/Dropbox/cWF_manuscript/Figs&amp;Supplementary_finalset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C834A69D-73B4-4BCC-82C6-4932D75CD3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6297D471-942A-C14D-869C-DCF420DA8A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13785" yWindow="-17490" windowWidth="30960" windowHeight="16800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="25360" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="mRNAvs.cWFs" sheetId="1" r:id="rId1"/>
+    <sheet name="Deconvolution_results" sheetId="1" r:id="rId1"/>
+    <sheet name="Celltype_abbreviation" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Deconvolution_results!$A$6:$B$15</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>B</t>
   </si>
@@ -34,10 +49,13 @@
     <t>DC</t>
   </si>
   <si>
+    <t>NK</t>
+  </si>
+  <si>
     <t>Neu</t>
   </si>
   <si>
-    <t>NK</t>
+    <t>Others</t>
   </si>
   <si>
     <t>PB</t>
@@ -46,20 +64,43 @@
     <t>T</t>
   </si>
   <si>
-    <t>cWFs mean of mean</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Signature genes#</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>RNA amount in the literature
-mRNA per cell [pg]</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>-</t>
+    <t>RMSE</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Pearson cor.</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Cell type</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Human PBMC</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>The optimal signature gene#</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Reference</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Signature genes #</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>T cells</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Plasmablasts</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Others (RBC, Platelet, Granulocytes etc.)</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
@@ -67,15 +108,35 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>Cell type</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>PBMC mRNA amount per cell vs. cWFs</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>cWFs SE of mean</t>
+    <t>Natural Killer cells</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Neutrophils</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Dendritic cells</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>CD16+ Monocytes</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>CD14+ Monocytes</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t xml:space="preserve">B cells </t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Cell type full name</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Abbreviation</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -83,14 +144,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.0000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000_ "/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -98,7 +160,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -106,7 +168,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="游ゴシック Light"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="major"/>
@@ -115,7 +177,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -124,7 +186,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -133,7 +195,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -141,7 +203,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -149,7 +211,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -157,7 +219,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -165,7 +227,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -174,7 +236,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -183,7 +245,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -191,7 +253,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -200,7 +262,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -208,7 +270,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -217,7 +279,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -226,7 +288,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -234,14 +296,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -249,6 +311,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -702,75 +770,84 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="6" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - アクセント 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - アクセント 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - アクセント 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - アクセント 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - アクセント 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - アクセント 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - アクセント 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - アクセント 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - アクセント 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - アクセント 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - アクセント 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - アクセント 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - アクセント 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - アクセント 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - アクセント 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - アクセント 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - アクセント 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - アクセント 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="アクセント 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="アクセント 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="アクセント 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="アクセント 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="アクセント 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="アクセント 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="タイトル" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="チェック セル" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="どちらでもない" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="メモ" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="リンク セル" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="悪い" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="計算" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="警告文" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="見出し 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="見出し 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="見出し 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="見出し 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="集計" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="出力" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="説明文" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="入力" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
-    <cellStyle name="良い" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -786,7 +863,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1082,405 +1159,382 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.09765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.59765625" style="2" customWidth="1"/>
-    <col min="3" max="5" width="8.796875" style="2"/>
-    <col min="6" max="6" width="2.8984375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.796875" style="2"/>
+    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="11" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="1"/>
+    <col min="7" max="7" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="C2" s="7" t="s">
+      <c r="C6" s="8">
+        <v>100</v>
+      </c>
+      <c r="D6" s="9">
+        <v>300</v>
+      </c>
+      <c r="E6" s="9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="4">
+        <v>5.8099999999999999E-2</v>
+      </c>
+      <c r="C7" s="5">
+        <v>3.8408194200976901E-2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.3298723118292E-2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1.7485918627244901E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.2001</v>
+      </c>
+      <c r="C8" s="5">
+        <v>4.7534502032157699E-2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>5.3063613216226102E-2</v>
+      </c>
+      <c r="E8" s="4">
+        <v>5.8580636267575502E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4">
+        <v>7.2099999999999997E-2</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2.76104436479057E-2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.10136799449447299</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.09867458643677E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="C10" s="5">
+        <v>3.7978715891506698E-2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>7.3368212393953199E-3</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1.0420259630187501E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4">
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.102428411254062</v>
+      </c>
+      <c r="D11" s="4">
+        <v>9.6074200235970499E-3</v>
+      </c>
+      <c r="E11" s="4">
+        <v>9.1750320070931295E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="4">
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.121843932704566</v>
+      </c>
+      <c r="D12" s="4">
+        <v>6.3554101116812201E-2</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3.2362471977273703E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4">
+        <v>3.7699999999999997E-2</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.11783009531158101</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.14142560291338999</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.14892919673416</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="4">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.117025080502521</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.39199842052399497</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.28284616949948599</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="G2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="C3" s="6" t="s">
+      <c r="B15" s="4">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.38934062445472301</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.21834730335381899</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.42921356939261202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="G3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="C17" s="6">
+        <v>9.2533203633847011E-2</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0.17894844222903944</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0.1199002785662746</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1">
-        <v>100</v>
-      </c>
-      <c r="D4" s="1">
-        <v>300</v>
-      </c>
-      <c r="E4" s="1">
-        <v>500</v>
-      </c>
-      <c r="G4" s="1">
-        <v>100</v>
-      </c>
-      <c r="H4" s="1">
-        <v>300</v>
-      </c>
-      <c r="I4" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0.347810768559071</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0.89031537515605097</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0.960733232652626</v>
-      </c>
-      <c r="G5" s="5">
-        <v>8.9444477229656497E-2</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0.239663726889527</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0.24724234990910501</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="C6" s="5">
-        <v>2.0269686499681301</v>
-      </c>
-      <c r="D6" s="5">
-        <v>2.0882486839831298</v>
-      </c>
-      <c r="E6" s="5">
-        <v>2.08958659283496</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0.22681550915173601</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0.22319396609782999</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0.21655597798892801</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0.40277542592913401</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1.2956722211174101</v>
-      </c>
-      <c r="E7" s="5">
-        <v>1.2319983437028801</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0.21450267463956599</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0.41508192703982699</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0.36749699490479298</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="5">
-        <v>3.8036600721934901</v>
-      </c>
-      <c r="D8" s="5">
-        <v>5.4692598961582704</v>
-      </c>
-      <c r="E8" s="5">
-        <v>5.4782618112769699</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0.769719610833001</v>
-      </c>
-      <c r="H8" s="5">
-        <v>1.2384765034279199</v>
-      </c>
-      <c r="I8" s="5">
-        <v>1.16986170679682</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.13</v>
-      </c>
-      <c r="C9" s="5">
-        <v>9.7196062920113402E-4</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0.33406214654632599</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.410979998473404</v>
-      </c>
-      <c r="G9" s="5">
-        <v>1.01288380919725E-4</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0.33276396210582698</v>
-      </c>
-      <c r="I9" s="5">
-        <v>0.409813884571049</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="C10" s="5">
-        <v>2.9677536061249999E-2</v>
-      </c>
-      <c r="D10" s="5">
-        <v>8.8103455217966295E-2</v>
-      </c>
-      <c r="E10" s="5">
-        <v>9.5495066650962496E-2</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1.8136773028867001E-2</v>
-      </c>
-      <c r="H10" s="5">
-        <v>4.2015618358294399E-2</v>
-      </c>
-      <c r="I10" s="5">
-        <v>4.4395721071883297E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="5">
-        <v>2.6603101254597301</v>
-      </c>
-      <c r="D11" s="5">
-        <v>2.79947948595875</v>
-      </c>
-      <c r="E11" s="5">
-        <v>2.7132181113178699</v>
-      </c>
-      <c r="G11" s="5">
-        <v>0.65998153250185099</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0.71052469188686296</v>
-      </c>
-      <c r="I11" s="5">
-        <v>0.66382929812777203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="5">
-        <v>1.0253504735755199E-3</v>
-      </c>
-      <c r="D12" s="5">
-        <v>1.1961802776372301E-3</v>
-      </c>
-      <c r="E12" s="5">
-        <v>1.09106992535061E-3</v>
-      </c>
-      <c r="G12" s="5">
-        <v>2.82895935187462E-4</v>
-      </c>
-      <c r="H12" s="5">
-        <v>3.1500994894707402E-4</v>
-      </c>
-      <c r="I12" s="5">
-        <v>2.7638846489113901E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0.28918932419787202</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0.57159974756108101</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.54841772996904803</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0.10943934955038501</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0.15325537853222099</v>
-      </c>
-      <c r="I13" s="5">
-        <v>0.14206626076509599</v>
+      <c r="C18" s="6">
+        <v>0.83657065402706554</v>
+      </c>
+      <c r="D18" s="6">
+        <f>CORREL(B7:B15,D7:D15)</f>
+        <v>0.20614022465751428</v>
+      </c>
+      <c r="E18" s="6">
+        <f>CORREL(B7:B15,E7:E15)</f>
+        <v>0.69110984332077341</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G3:I3"/>
+  <mergeCells count="1">
+    <mergeCell ref="C5:E5"/>
   </mergeCells>
   <phoneticPr fontId="18"/>
-  <conditionalFormatting sqref="C5:C13">
-    <cfRule type="dataBar" priority="3">
+  <conditionalFormatting sqref="B7:E15">
+    <cfRule type="dataBar" priority="1">
       <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
         <color rgb="FF008AEF"/>
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{995E7559-45B6-44D1-A0FF-CAF1E0554B14}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D13">
-    <cfRule type="dataBar" priority="2">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFB628"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{682718E5-AE5B-4F0E-BEAE-13712774844D}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5:E13">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFD6007B"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{96CCE200-A563-41C0-96BA-A6DD6E4E67BC}</x14:id>
+          <x14:id>{F9B9F61F-7A3F-4984-98E7-D31DE2CC51EA}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{995E7559-45B6-44D1-A0FF-CAF1E0554B14}">
+          <x14:cfRule type="dataBar" id="{F9B9F61F-7A3F-4984-98E7-D31DE2CC51EA}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
               <x14:borderColor rgb="FF008AEF"/>
               <x14:negativeFillColor rgb="FFFF0000"/>
               <x14:negativeBorderColor rgb="FFFF0000"/>
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C5:C13</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{682718E5-AE5B-4F0E-BEAE-13712774844D}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FFFFB628"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D5:D13</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{96CCE200-A563-41C0-96BA-A6DD6E4E67BC}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FFD6007B"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E5:E13</xm:sqref>
+          <xm:sqref>B7:E15</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34A90AC3-F00C-4CD0-AF83-5177D7C9960E}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>